<commit_message>
updated TODO for current sprint
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wucki\Desktop\Projects\5.Klasse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8148"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Funktionalität</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Mitarbeiter(mit jeweiliger Rolle) anlegen</t>
   </si>
   <si>
-    <t>Beim Mitarbeiter Anlegen kann man seine Rolle auswählen</t>
-  </si>
-  <si>
     <t>Rollen hinzufügen</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>Stays anzeigen</t>
   </si>
   <si>
-    <t>Von/Bis: Datum funktioniert nicht</t>
-  </si>
-  <si>
     <t>Alle Stays werden angezeigt</t>
   </si>
   <si>
@@ -108,12 +102,42 @@
   </si>
   <si>
     <t>Rolle hinzufügen können hinzugefügt werden</t>
+  </si>
+  <si>
+    <t>Als Administrator kann man Mitarbeiter hinzufügen/ändern/löschen</t>
+  </si>
+  <si>
+    <t>Anzeige für den Koch gestalten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koch kann sich anmelden, alle offenen Bestellungen einsehen, diese aktualiesieren sich alle 5 Sekunden und diese nach zubereitung auf "gemacht" setzen </t>
+  </si>
+  <si>
+    <t>Admin Fenster erweitern</t>
+  </si>
+  <si>
+    <t>Admin hat nun die Möglichkeit Speißen hinzuzufügen, bearbeiten, löschen</t>
+  </si>
+  <si>
+    <t>Anzeige für Barkeeper gestalten</t>
+  </si>
+  <si>
+    <t>Barkeeper kann sich anmelden, alle offen Zimmerservicebestellungen einsehen, diese aktualisieren sich alle 5 Sekunden und diese nach Zubereitung auf "fertig" setzen.</t>
+  </si>
+  <si>
+    <t>Anwendung vollständig auf WebServices umstellen</t>
+  </si>
+  <si>
+    <t>Jeglicher Datenbankzugriff soll mittels WebService funktionieren.</t>
+  </si>
+  <si>
+    <t>Alles wurde erfolgreich umgstellt, steckt jedoch noch in der Testphase.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -259,7 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -350,6 +374,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -385,6 +426,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,17 +598,17 @@
   <dimension ref="A3:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="83.28515625" customWidth="1"/>
+    <col min="2" max="2" width="83.33203125" customWidth="1"/>
     <col min="4" max="4" width="72" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -567,16 +625,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -591,7 +649,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -599,193 +657,217 @@
         <v>7</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
       <c r="B17" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>1</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>2</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>3</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>4</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>5</v>
       </c>
@@ -794,7 +876,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -803,7 +885,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>7</v>
       </c>
@@ -812,7 +894,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>8</v>
       </c>
@@ -821,7 +903,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>9</v>
       </c>
@@ -830,7 +912,7 @@
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>10</v>
       </c>
@@ -839,7 +921,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>11</v>
       </c>
@@ -848,7 +930,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>12</v>
       </c>
@@ -857,7 +939,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>13</v>
       </c>
@@ -866,7 +948,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>14</v>
       </c>
@@ -875,7 +957,7 @@
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>15</v>
       </c>
@@ -884,7 +966,7 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>16</v>
       </c>

</xml_diff>